<commit_message>
fix schematics and BOMs
</commit_message>
<xml_diff>
--- a/boards/Bridge/Bridge_BOM.xlsx
+++ b/boards/Bridge/Bridge_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lipoy\Dropbox\develop\StackChanPwd\StackChanPwd\boards\Bridge\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{FFC92555-E9C3-4740-8DC1-CFBAFFB5A3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DF030D8-8D27-4C96-B743-51ACE77C96AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{4109BE55-E47C-4ADB-8DD7-B48545A95EEA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{4109BE55-E47C-4ADB-8DD7-B48545A95EEA}"/>
   </bookViews>
   <sheets>
     <sheet name="Bridge_BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="63">
   <si>
     <t>Reference</t>
   </si>
@@ -95,12 +95,6 @@
   </si>
   <si>
     <t>CN4,CN5</t>
-  </si>
-  <si>
-    <t>1x3 PinHeader</t>
-  </si>
-  <si>
-    <t>サーボ用</t>
   </si>
   <si>
     <t>CN6</t>
@@ -204,6 +198,21 @@
   </si>
   <si>
     <t>490-GRM31CR61A107MEA8KCT-ND</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>B3B-EH-A</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>EH 3ピン (トップ型)</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>455-B3B-EH-A-ND</t>
     <phoneticPr fontId="18"/>
   </si>
 </sst>
@@ -824,7 +833,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -836,6 +845,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1194,7 +1206,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87F13F83-DDCA-486F-832B-CFC234E04F22}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
@@ -1263,7 +1277,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>10</v>
@@ -1271,10 +1285,10 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1361,37 +1375,37 @@
         <v>2</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>26</v>
+        <v>61</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>11</v>
+        <v>48</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1" t="s">
@@ -1403,19 +1417,19 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B9" s="3">
         <v>2</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>5</v>
@@ -1429,21 +1443,21 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B10" s="1">
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H10" s="1">
         <v>102073</v>
@@ -1451,21 +1465,21 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1">
         <v>3</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H11" s="1">
         <v>110191</v>
@@ -1473,13 +1487,13 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1">
         <v>2</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
@@ -1495,13 +1509,13 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>10</v>
@@ -1517,23 +1531,23 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B14" s="3">
         <v>1</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H14" s="3">
         <v>107591</v>
@@ -1541,72 +1555,72 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>49</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B17" s="1">
         <v>1</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>